<commit_message>
add main diplom file
</commit_message>
<xml_diff>
--- a/economy/data.xlsx
+++ b/economy/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSUIR\diplom\economic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Документы\Учеба\4 курс\Диплом\diplom\economy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -190,19 +190,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,7 +487,7 @@
   <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,48 +499,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>6</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>7</v>
       </c>
     </row>
@@ -623,50 +623,50 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="2"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="6"/>
-      <c r="D17" s="5">
+      <c r="C17" s="7"/>
+      <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>3</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>4</v>
       </c>
     </row>
@@ -707,7 +707,7 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2"/>
@@ -725,7 +725,7 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="2"/>
@@ -734,7 +734,7 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="2"/>
@@ -752,47 +752,47 @@
       <c r="G26" s="2"/>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>1</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="3:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D36" s="2"/>

</xml_diff>